<commit_message>
fix the name  product problem
</commit_message>
<xml_diff>
--- a/Search Products/CommanNotFoundFile.xlsx
+++ b/Search Products/CommanNotFoundFile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>Title</t>
   </si>
@@ -25,6 +25,9 @@
     <t>NH8350-83AB</t>
   </si>
   <si>
+    <t>NB6021-68L</t>
+  </si>
+  <si>
     <t>FE7040-53E</t>
   </si>
   <si>
@@ -58,12 +61,18 @@
     <t>EQ0593-26A</t>
   </si>
   <si>
+    <t>EM0504-81A</t>
+  </si>
+  <si>
     <t>BN0225-04L</t>
   </si>
   <si>
     <t>BM7462-15E</t>
   </si>
   <si>
+    <t>BM7407-81H</t>
+  </si>
+  <si>
     <t>BI5104-57Z</t>
   </si>
   <si>
@@ -97,6 +106,9 @@
     <t>BI5000-87A</t>
   </si>
   <si>
+    <t>BI1050-81E</t>
+  </si>
+  <si>
     <t>BH5002-53E</t>
   </si>
   <si>
@@ -127,15 +139,72 @@
     <t>AK5003-05A</t>
   </si>
   <si>
+    <t>SFJ005J1</t>
+  </si>
+  <si>
+    <t>SFJ007J1</t>
+  </si>
+  <si>
+    <t>SFQ801P1</t>
+  </si>
+  <si>
+    <t>SFQ803P1</t>
+  </si>
+  <si>
+    <t>SGEH85P1</t>
+  </si>
+  <si>
+    <t>SNDH31P1</t>
+  </si>
+  <si>
+    <t>SNDH47P1</t>
+  </si>
+  <si>
+    <t>SNDV34P1</t>
+  </si>
+  <si>
+    <t>SNE498P1</t>
+  </si>
+  <si>
+    <t>SNE541P1</t>
+  </si>
+  <si>
+    <t>SNE543P1</t>
+  </si>
+  <si>
+    <t>SNE549P1</t>
+  </si>
+  <si>
+    <t>SNE559P1</t>
+  </si>
+  <si>
+    <t>SNE573P1</t>
+  </si>
+  <si>
+    <t>SNJ028P1</t>
+  </si>
+  <si>
+    <t>SNJ031P1</t>
+  </si>
+  <si>
     <t>SNKD99K1</t>
   </si>
   <si>
+    <t>SNKE01K1</t>
+  </si>
+  <si>
     <t>SNKE04K1</t>
   </si>
   <si>
     <t>SNKE06K1</t>
   </si>
   <si>
+    <t>SNKE51K1</t>
+  </si>
+  <si>
+    <t>SNKE53K1</t>
+  </si>
+  <si>
     <t>SNKE54K1</t>
   </si>
   <si>
@@ -145,12 +214,30 @@
     <t>SNKK09K1</t>
   </si>
   <si>
+    <t>SNKK17K1</t>
+  </si>
+  <si>
+    <t>SNKK25K1</t>
+  </si>
+  <si>
+    <t>SNKK31K1</t>
+  </si>
+  <si>
     <t>SNKK67K1</t>
   </si>
   <si>
     <t>SNKK71K1</t>
   </si>
   <si>
+    <t>SNKL15K1</t>
+  </si>
+  <si>
+    <t>SNKL17K1</t>
+  </si>
+  <si>
+    <t>SNKL19K1</t>
+  </si>
+  <si>
     <t>SNKL23K1</t>
   </si>
   <si>
@@ -175,10 +262,295 @@
     <t>SNKL57K1</t>
   </si>
   <si>
+    <t>SNKL58K1</t>
+  </si>
+  <si>
     <t>SNKL79K1</t>
   </si>
   <si>
-    <t>SSK005K1(Orange)</t>
+    <t>SNKP17K1</t>
+  </si>
+  <si>
+    <t>SNKP20K1</t>
+  </si>
+  <si>
+    <t>SPB117J1</t>
+  </si>
+  <si>
+    <t>SPB157J1</t>
+  </si>
+  <si>
+    <t>SPB169J1</t>
+  </si>
+  <si>
+    <t>SPB191J1</t>
+  </si>
+  <si>
+    <t>SPB203J1</t>
+  </si>
+  <si>
+    <t>SPB209J1</t>
+  </si>
+  <si>
+    <t>SPB210J1</t>
+  </si>
+  <si>
+    <t>SPB213J1</t>
+  </si>
+  <si>
+    <t>SPB249J1</t>
+  </si>
+  <si>
+    <t>SPB381J1</t>
+  </si>
+  <si>
+    <t>SPB385J1</t>
+  </si>
+  <si>
+    <t>SRE006K1</t>
+  </si>
+  <si>
+    <t>SRKZ53P1</t>
+  </si>
+  <si>
+    <t>SRP839J1</t>
+  </si>
+  <si>
+    <t>SRP851P1</t>
+  </si>
+  <si>
+    <t>SRP856J1</t>
+  </si>
+  <si>
+    <t>SRPB44J1</t>
+  </si>
+  <si>
+    <t>SRPB46J1</t>
+  </si>
+  <si>
+    <t>SRPB47J1</t>
+  </si>
+  <si>
+    <t>SRPD21K1</t>
+  </si>
+  <si>
+    <t>SRPD23K1</t>
+  </si>
+  <si>
+    <t>SRPD25K1</t>
+  </si>
+  <si>
+    <t>SRPD29K1</t>
+  </si>
+  <si>
+    <t>SRPD69K1</t>
+  </si>
+  <si>
+    <t>SRPD97J1</t>
+  </si>
+  <si>
+    <t>SRPE07K1</t>
+  </si>
+  <si>
+    <t>SRPE41J1</t>
+  </si>
+  <si>
+    <t>SRPE43J1</t>
+  </si>
+  <si>
+    <t>SRPE85K1</t>
+  </si>
+  <si>
+    <t>SRPE87K1</t>
+  </si>
+  <si>
+    <t>SRPE91K1</t>
+  </si>
+  <si>
+    <t>SRPE95K1</t>
+  </si>
+  <si>
+    <t>SRPF07K1</t>
+  </si>
+  <si>
+    <t>SRPF15K1</t>
+  </si>
+  <si>
+    <t>SRPF25J1</t>
+  </si>
+  <si>
+    <t>SRPF47J1</t>
+  </si>
+  <si>
+    <t>SRPF49J1</t>
+  </si>
+  <si>
+    <t>SRPF81K1</t>
+  </si>
+  <si>
+    <t>SRPG03J1</t>
+  </si>
+  <si>
+    <t>SRPG39K1</t>
+  </si>
+  <si>
+    <t>SRPH25K1</t>
+  </si>
+  <si>
+    <t>SRPJ17J1</t>
+  </si>
+  <si>
+    <t>SRPJ79K1</t>
+  </si>
+  <si>
+    <t>SRPJ91K1</t>
+  </si>
+  <si>
+    <t>SRQ037J1</t>
+  </si>
+  <si>
+    <t>SRZ502P1</t>
+  </si>
+  <si>
+    <t>SRZ508P1</t>
+  </si>
+  <si>
+    <t>SRZ512P1</t>
+  </si>
+  <si>
+    <t>SRZ514P1</t>
+  </si>
+  <si>
+    <t>SSA399J1</t>
+  </si>
+  <si>
+    <t>SSA407J1</t>
+  </si>
+  <si>
+    <t>SSA423J1</t>
+  </si>
+  <si>
+    <t>SSA426J1</t>
+  </si>
+  <si>
+    <t>SSA441J1</t>
+  </si>
+  <si>
+    <t>SSB375P1</t>
+  </si>
+  <si>
+    <t>SSB380P1</t>
+  </si>
+  <si>
+    <t>SSC779P1</t>
+  </si>
+  <si>
+    <t>SSC781P1</t>
+  </si>
+  <si>
+    <t>SSC783P1</t>
+  </si>
+  <si>
+    <t>SSC785P1</t>
+  </si>
+  <si>
+    <t>SUR237P1</t>
+  </si>
+  <si>
+    <t>SUR266P1</t>
+  </si>
+  <si>
+    <t>SUR284P1</t>
+  </si>
+  <si>
+    <t>SUR299P1</t>
+  </si>
+  <si>
+    <t>SUR306P1</t>
+  </si>
+  <si>
+    <t>SUR314P1</t>
+  </si>
+  <si>
+    <t>SUR317P1</t>
+  </si>
+  <si>
+    <t>SUR330P1</t>
+  </si>
+  <si>
+    <t>SUR339P1</t>
+  </si>
+  <si>
+    <t>SUR341P1</t>
+  </si>
+  <si>
+    <t>SUR347P1</t>
+  </si>
+  <si>
+    <t>SUR348P1</t>
+  </si>
+  <si>
+    <t>SUR379P1</t>
+  </si>
+  <si>
+    <t>SUR380P1</t>
+  </si>
+  <si>
+    <t>SUR385P1</t>
+  </si>
+  <si>
+    <t>SUR399P1</t>
+  </si>
+  <si>
+    <t>SUR402P1</t>
+  </si>
+  <si>
+    <t>SUR404P1</t>
+  </si>
+  <si>
+    <t>SUR412P1</t>
+  </si>
+  <si>
+    <t>SUR456P1</t>
+  </si>
+  <si>
+    <t>SUR460P1</t>
+  </si>
+  <si>
+    <t>SUR461P1</t>
+  </si>
+  <si>
+    <t>SUR470P1</t>
+  </si>
+  <si>
+    <t>SUR474P1</t>
+  </si>
+  <si>
+    <t>SUR479P1</t>
+  </si>
+  <si>
+    <t>SUR538P1</t>
+  </si>
+  <si>
+    <t>SUR542P1</t>
+  </si>
+  <si>
+    <t>SUR632P1</t>
+  </si>
+  <si>
+    <t>SUR634P1</t>
+  </si>
+  <si>
+    <t>SUT403P1</t>
+  </si>
+  <si>
+    <t>SUT405P1</t>
+  </si>
+  <si>
+    <t>SWR035P1</t>
+  </si>
+  <si>
+    <t>SWR073P1</t>
   </si>
 </sst>
 </file>
@@ -555,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A56"/>
+  <dimension ref="A1:A180"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -838,6 +1210,626 @@
         <v>55</v>
       </c>
     </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>